<commit_message>
added data to the sample data
</commit_message>
<xml_diff>
--- a/src/test/resources/Recommender Math.xlsx
+++ b/src/test/resources/Recommender Math.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="0" windowWidth="25380" windowHeight="17480" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="260" yWindow="0" windowWidth="25380" windowHeight="17480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix Math" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="51">
   <si>
     <t>user/item</t>
   </si>
@@ -126,7 +126,7 @@
     <t>surface</t>
   </si>
   <si>
-    <t>nexus-tablet</t>
+    <t>iphone, ipad</t>
   </si>
   <si>
     <t>Recommendations</t>
@@ -136,6 +136,45 @@
   </si>
   <si>
     <t>Table</t>
+  </si>
+  <si>
+    <t>Cross-action Recommendations</t>
+  </si>
+  <si>
+    <t>iphone, galaxy, ipad, nexus</t>
+  </si>
+  <si>
+    <t>galaxy, nexus</t>
+  </si>
+  <si>
+    <t>Cross-action Similari Items</t>
+  </si>
+  <si>
+    <t>galaxy, ipad, nexus</t>
+  </si>
+  <si>
+    <t>iphone, galaxy, nexus</t>
+  </si>
+  <si>
+    <t>iphone, galaxy, ipad</t>
+  </si>
+  <si>
+    <t>iphone, ipad, nexus</t>
+  </si>
+  <si>
+    <t>columns of [B'A]</t>
+  </si>
+  <si>
+    <t>rows of [B'A]</t>
+  </si>
+  <si>
+    <t>ipad, nexus, galaxy</t>
+  </si>
+  <si>
+    <t>iphone, nexus, galaxy</t>
+  </si>
+  <si>
+    <t>iphone, ipad, galaxy</t>
   </si>
 </sst>
 </file>
@@ -202,8 +241,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="129">
+  <cellStyleXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -353,11 +406,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="129">
+  <cellStyles count="143">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -422,6 +475,13 @@
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -486,6 +546,13 @@
     <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -874,10 +941,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q62"/>
+  <dimension ref="A1:Q76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M42" sqref="M42:M53"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1575,7 +1642,7 @@
         <v>0</v>
       </c>
       <c r="E38" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" s="4">
         <v>0</v>
@@ -1679,7 +1746,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F44" s="3">
         <v>1</v>
@@ -1843,7 +1910,7 @@
         <v>0</v>
       </c>
       <c r="E53" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" s="3">
         <v>0</v>
@@ -1920,7 +1987,7 @@
         <v>7</v>
       </c>
       <c r="G56" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J56" t="s">
         <v>20</v>
@@ -1936,7 +2003,7 @@
         <v>7</v>
       </c>
       <c r="P56" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q56" s="3">
         <v>6</v>
@@ -1959,7 +2026,7 @@
         <v>7</v>
       </c>
       <c r="G57" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M57" s="2" t="s">
         <v>30</v>
@@ -1971,7 +2038,7 @@
         <v>4</v>
       </c>
       <c r="P57" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q57" s="3">
         <v>3</v>
@@ -1982,19 +2049,19 @@
         <v>3</v>
       </c>
       <c r="C58" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D58" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E58" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F58" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G58" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M58" s="2" t="s">
         <v>31</v>
@@ -2006,7 +2073,7 @@
         <v>4</v>
       </c>
       <c r="P58" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q58" s="3">
         <v>3</v>
@@ -2029,7 +2096,7 @@
         <v>6</v>
       </c>
       <c r="G59" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M59" s="2" t="s">
         <v>32</v>
@@ -2041,7 +2108,7 @@
         <v>7</v>
       </c>
       <c r="P59" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q59" s="3">
         <v>6</v>
@@ -2052,27 +2119,151 @@
         <v>33</v>
       </c>
       <c r="N60" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O60" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P60" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q60" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:17">
-      <c r="B61" s="7"/>
+      <c r="A61" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="62" spans="1:17">
-      <c r="B62" s="7"/>
+      <c r="A62" s="7"/>
+      <c r="B62" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17">
+      <c r="B63" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17">
+      <c r="B64" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C66" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="7"/>
+      <c r="B67" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C67" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>46</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C68" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="B69" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C69" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="B70" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C72" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="7"/>
+      <c r="B73" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C73" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>47</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C74" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="B75" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C75" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="B76" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C76" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="B1:G1"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="A72:A73"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2086,10 +2277,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2124,7 +2315,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2201,7 +2392,7 @@
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2245,7 +2436,7 @@
         <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2272,13 +2463,13 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
         <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2289,7 +2480,7 @@
         <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2300,11 +2491,23 @@
         <v>28</v>
       </c>
       <c r="C19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
took out downsampling rather than integrate with new RecommenderJob and other refactored code
</commit_message>
<xml_diff>
--- a/src/test/resources/Recommender Math.xlsx
+++ b/src/test/resources/Recommender Math.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="61">
   <si>
     <t>user/item</t>
   </si>
@@ -126,6 +126,15 @@
     <t>surface</t>
   </si>
   <si>
+    <t>Key: 0: Value: {0:1.0,1:1.0}</t>
+  </si>
+  <si>
+    <t>Key: 1: Value: {3:1.0,2:1.0}</t>
+  </si>
+  <si>
+    <t>Key: 2: Value: {4:1.0}</t>
+  </si>
+  <si>
     <t>Recommendations</t>
   </si>
   <si>
@@ -181,6 +190,21 @@
   </si>
   <si>
     <t>Cross-action Similar Items</t>
+  </si>
+  <si>
+    <t>Key: 3: Value: {0:1.0,3:1.0}</t>
+  </si>
+  <si>
+    <t>Key: 0: Value: {0:1.0,1:1.0,2:1.0,3:1.0}</t>
+  </si>
+  <si>
+    <t>Key: 1: Value: {0:1.0,1:1.0,2:1.0,3:1.0}</t>
+  </si>
+  <si>
+    <t>Key: 2: Value: {4:1.0,2:1.0}</t>
+  </si>
+  <si>
+    <t>Key: 3: Value: {0:1.0,1:1.0,3:1.0}</t>
   </si>
 </sst>
 </file>
@@ -904,7 +928,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="44" customHeight="1">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>11</v>
@@ -949,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -958,7 +982,7 @@
     <col min="1" max="1" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -974,7 +998,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1000,7 +1024,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:14">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1019,8 +1043,11 @@
       <c r="G3" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="N3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1039,8 +1066,11 @@
       <c r="G4" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="N4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1059,8 +1089,11 @@
       <c r="G5" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="N5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1079,8 +1112,11 @@
       <c r="G6" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="N6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1103,7 +1139,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:14">
       <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
@@ -1121,7 +1157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:14">
       <c r="B10" s="2" t="s">
         <v>30</v>
       </c>
@@ -1138,7 +1174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:14">
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
@@ -1155,7 +1191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:14">
       <c r="B12" s="2" t="s">
         <v>32</v>
       </c>
@@ -1172,7 +1208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:14">
       <c r="B13" s="2" t="s">
         <v>33</v>
       </c>
@@ -1189,7 +1225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1221,7 +1257,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:14">
       <c r="B16" s="2" t="s">
         <v>29</v>
       </c>
@@ -1536,7 +1572,7 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>1</v>
@@ -1563,15 +1599,15 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -1597,7 +1633,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:14">
       <c r="B36" s="1" t="s">
         <v>1</v>
       </c>
@@ -1616,8 +1652,11 @@
       <c r="G36" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:11">
+      <c r="N36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="B37" s="1" t="s">
         <v>2</v>
       </c>
@@ -1636,8 +1675,11 @@
       <c r="G37" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:11">
+      <c r="N37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="B38" s="1" t="s">
         <v>3</v>
       </c>
@@ -1656,8 +1698,11 @@
       <c r="G38" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:11">
+      <c r="N38" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="B39" s="1" t="s">
         <v>4</v>
       </c>
@@ -1668,16 +1713,19 @@
         <v>1</v>
       </c>
       <c r="E39" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F39" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:11">
+      <c r="N39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -1706,7 +1754,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:14">
       <c r="B42" s="2" t="s">
         <v>29</v>
       </c>
@@ -1724,7 +1772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:14">
       <c r="B43" s="2" t="s">
         <v>30</v>
       </c>
@@ -1741,7 +1789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:14">
       <c r="B44" s="2" t="s">
         <v>31</v>
       </c>
@@ -1755,10 +1803,10 @@
         <v>1</v>
       </c>
       <c r="F44" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
       <c r="B45" s="2" t="s">
         <v>32</v>
       </c>
@@ -1772,10 +1820,10 @@
         <v>0</v>
       </c>
       <c r="F45" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
       <c r="B46" s="2" t="s">
         <v>33</v>
       </c>
@@ -1792,13 +1840,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:14">
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:14">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -1836,10 +1884,10 @@
         <v>2</v>
       </c>
       <c r="E49" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G49" s="3">
         <v>0</v>
@@ -1896,10 +1944,10 @@
         <v>2</v>
       </c>
       <c r="E52" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G52" s="3">
         <v>0</v>
@@ -2009,7 +2057,7 @@
         <v>7</v>
       </c>
       <c r="P56" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q56" s="3">
         <v>6</v>
@@ -2055,7 +2103,7 @@
         <v>3</v>
       </c>
       <c r="C58" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D58" s="3">
         <v>1</v>
@@ -2064,7 +2112,7 @@
         <v>1</v>
       </c>
       <c r="F58" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G58" s="3">
         <v>2</v>
@@ -2102,7 +2150,7 @@
         <v>6</v>
       </c>
       <c r="G59" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M59" s="2" t="s">
         <v>32</v>
@@ -2114,7 +2162,7 @@
         <v>7</v>
       </c>
       <c r="P59" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q59" s="3">
         <v>6</v>
@@ -2134,18 +2182,18 @@
         <v>2</v>
       </c>
       <c r="Q60" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:17">
       <c r="A61" s="7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="62" spans="1:17">
@@ -2154,7 +2202,7 @@
         <v>2</v>
       </c>
       <c r="C62" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="63" spans="1:17">
@@ -2165,7 +2213,7 @@
         <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:17">
@@ -2173,18 +2221,18 @@
         <v>4</v>
       </c>
       <c r="C64" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C66" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -2193,18 +2241,18 @@
         <v>30</v>
       </c>
       <c r="C67" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C68" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -2212,7 +2260,7 @@
         <v>32</v>
       </c>
       <c r="C69" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -2222,13 +2270,13 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="7" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C72" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -2237,18 +2285,18 @@
         <v>30</v>
       </c>
       <c r="C73" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C74" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2256,7 +2304,7 @@
         <v>32</v>
       </c>
       <c r="C75" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="1:3">

</xml_diff>

<commit_message>
adding in some options that weren't completely implemented. Can pass in the actions strings to look for now
</commit_message>
<xml_diff>
--- a/src/test/resources/Recommender Math.xlsx
+++ b/src/test/resources/Recommender Math.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="0" windowWidth="25380" windowHeight="17480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="260" yWindow="40" windowWidth="28500" windowHeight="17480" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix Math" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="63">
   <si>
     <t>user/item</t>
   </si>
@@ -78,9 +78,6 @@
     <t>B'A</t>
   </si>
   <si>
-    <t>[[B'B]H_b]'</t>
-  </si>
-  <si>
     <t>*[5x4]=</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>A' = H_a</t>
   </si>
   <si>
-    <t>B' = H_b</t>
-  </si>
-  <si>
     <t>[[B'A]H_a]</t>
   </si>
   <si>
@@ -141,9 +135,6 @@
     <t>ipad, nexus</t>
   </si>
   <si>
-    <t>Table</t>
-  </si>
-  <si>
     <t>Cross-action Recommendations</t>
   </si>
   <si>
@@ -205,12 +196,30 @@
   </si>
   <si>
     <t>Key: 3: Value: {0:1.0,1:1.0,3:1.0}</t>
+  </si>
+  <si>
+    <t>userID</t>
+  </si>
+  <si>
+    <t>itemID</t>
+  </si>
+  <si>
+    <t>preference</t>
+  </si>
+  <si>
+    <t>B' = H_p</t>
+  </si>
+  <si>
+    <t>[[B'B]H_p]'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -262,7 +271,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -270,8 +279,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="143">
+  <cellStyleXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -415,8 +433,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -439,8 +485,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="143">
+  <cellStyles count="171">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -512,6 +560,20 @@
     <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -583,6 +645,20 @@
     <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -912,10 +988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G31"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -926,9 +1002,9 @@
     <col min="10" max="10" width="7.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="44" customHeight="1">
+    <row r="1" spans="1:16" ht="44" customHeight="1">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>11</v>
@@ -940,20 +1016,575 @@
       <c r="G1" s="6"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="I2" s="5"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="3" spans="1:16">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="I8" s="5"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="9" spans="1:16">
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <f t="array" ref="C9:F13">TRANSPOSE(C3:G6)</f>
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="B10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="B11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="B13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-    </row>
-    <row r="22" spans="9:11">
+      <c r="K15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="B16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16">
+        <f t="array" ref="C16:G20">MMULT(C9:F13,C3:G6)</f>
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M16">
+        <f t="array" ref="M16:P20">MMULT(C16:G20,C9:F13)</f>
+        <v>3</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="B17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M17">
+        <v>2</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="B18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>2</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="B19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>3</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="B20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="B23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <f t="array" ref="C23:G26">TRANSPOSE(M16:P20)</f>
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="B24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="B29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="B30" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="B31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -973,8 +1604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1006,19 +1637,19 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>7</v>
@@ -1044,7 +1675,7 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -1067,7 +1698,7 @@
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -1090,7 +1721,7 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -1113,12 +1744,12 @@
         <v>0</v>
       </c>
       <c r="N6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
@@ -1141,7 +1772,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" s="3">
         <f t="array" ref="C9:F13">TRANSPOSE(C3:G6)</f>
@@ -1159,7 +1790,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="B10" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
@@ -1176,7 +1807,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="B11" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" s="3">
         <v>0</v>
@@ -1193,7 +1824,7 @@
     </row>
     <row r="12" spans="1:14">
       <c r="B12" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12" s="3">
         <v>0</v>
@@ -1210,7 +1841,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="B13" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13" s="3">
         <v>0</v>
@@ -1233,19 +1864,19 @@
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>8</v>
@@ -1259,7 +1890,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C16" s="3">
         <f t="array" ref="C16:G20">MMULT(C9:F13,C3:G6)</f>
@@ -1280,7 +1911,7 @@
     </row>
     <row r="17" spans="1:17">
       <c r="B17" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
@@ -1300,7 +1931,7 @@
     </row>
     <row r="18" spans="1:17">
       <c r="B18" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C18" s="3">
         <v>0</v>
@@ -1320,7 +1951,7 @@
     </row>
     <row r="19" spans="1:17">
       <c r="B19" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>
@@ -1340,7 +1971,7 @@
     </row>
     <row r="20" spans="1:17">
       <c r="B20" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
@@ -1360,37 +1991,37 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>12</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>8</v>
       </c>
       <c r="L22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M22" s="1" t="s">
         <v>15</v>
@@ -1429,10 +2060,10 @@
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N23" s="3">
         <f t="array" ref="N23:Q27">MMULT(C16:G20, C9:F13)</f>
@@ -1468,7 +2099,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N24" s="3">
         <v>2</v>
@@ -1503,7 +2134,7 @@
         <v>1</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="N25" s="3">
         <v>0</v>
@@ -1538,7 +2169,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N26" s="3">
         <v>1</v>
@@ -1555,7 +2186,7 @@
     </row>
     <row r="27" spans="1:17">
       <c r="M27" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="N27" s="3">
         <v>0</v>
@@ -1572,13 +2203,13 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -1586,7 +2217,7 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -1599,12 +2230,12 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:14">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -1615,19 +2246,19 @@
         <v>0</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>7</v>
@@ -1653,7 +2284,7 @@
         <v>0</v>
       </c>
       <c r="N36" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -1676,7 +2307,7 @@
         <v>0</v>
       </c>
       <c r="N37" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:14">
@@ -1699,7 +2330,7 @@
         <v>1</v>
       </c>
       <c r="N38" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:14">
@@ -1722,12 +2353,12 @@
         <v>0</v>
       </c>
       <c r="N39" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:14">
       <c r="A41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>15</v>
@@ -1756,7 +2387,7 @@
     </row>
     <row r="42" spans="1:14">
       <c r="B42" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C42" s="3">
         <f t="array" ref="C42:F46">TRANSPOSE(C36:G39)</f>
@@ -1774,7 +2405,7 @@
     </row>
     <row r="43" spans="1:14">
       <c r="B43" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C43" s="3">
         <v>1</v>
@@ -1791,7 +2422,7 @@
     </row>
     <row r="44" spans="1:14">
       <c r="B44" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C44" s="3">
         <v>1</v>
@@ -1808,7 +2439,7 @@
     </row>
     <row r="45" spans="1:14">
       <c r="B45" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C45" s="3">
         <v>1</v>
@@ -1825,7 +2456,7 @@
     </row>
     <row r="46" spans="1:14">
       <c r="B46" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C46" s="3">
         <v>0</v>
@@ -1854,19 +2485,19 @@
         <v>14</v>
       </c>
       <c r="C48" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="G48" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="I48" s="5" t="s">
         <v>12</v>
@@ -1874,7 +2505,7 @@
     </row>
     <row r="49" spans="1:17">
       <c r="B49" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C49" s="3">
         <f t="array" ref="C49:G53">MMULT(C9:F13,C36:G39)</f>
@@ -1895,7 +2526,7 @@
     </row>
     <row r="50" spans="1:17">
       <c r="B50" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C50" s="3">
         <v>1</v>
@@ -1915,7 +2546,7 @@
     </row>
     <row r="51" spans="1:17">
       <c r="B51" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C51" s="3">
         <v>1</v>
@@ -1935,7 +2566,7 @@
     </row>
     <row r="52" spans="1:17">
       <c r="B52" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C52" s="3">
         <v>2</v>
@@ -1955,7 +2586,7 @@
     </row>
     <row r="53" spans="1:17">
       <c r="B53" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C53" s="3">
         <v>0</v>
@@ -1975,37 +2606,37 @@
     </row>
     <row r="55" spans="1:17">
       <c r="A55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C55" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="G55" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="I55" s="3" t="s">
         <v>12</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K55" s="3" t="s">
         <v>8</v>
       </c>
       <c r="L55" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M55" s="1" t="s">
         <v>15</v>
@@ -2044,10 +2675,10 @@
         <v>1</v>
       </c>
       <c r="J56" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N56" s="3">
         <f t="array" ref="N56:Q60">MMULT(C49:G53,C42:F46)</f>
@@ -2083,7 +2714,7 @@
         <v>1</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N57" s="3">
         <v>4</v>
@@ -2118,7 +2749,7 @@
         <v>2</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="N58" s="3">
         <v>4</v>
@@ -2153,7 +2784,7 @@
         <v>0</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N59" s="3">
         <v>7</v>
@@ -2170,7 +2801,7 @@
     </row>
     <row r="60" spans="1:17">
       <c r="M60" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="N60" s="3">
         <v>1</v>
@@ -2187,13 +2818,13 @@
     </row>
     <row r="61" spans="1:17">
       <c r="A61" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="62" spans="1:17">
@@ -2202,18 +2833,18 @@
         <v>2</v>
       </c>
       <c r="C62" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="63" spans="1:17">
       <c r="A63" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:17">
@@ -2221,98 +2852,98 @@
         <v>4</v>
       </c>
       <c r="C64" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C66" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="7"/>
       <c r="B67" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C67" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C68" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="B69" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C69" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="B70" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C72" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="7"/>
       <c r="B73" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C73" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
+        <v>44</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C74" t="s">
         <v>47</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C74" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="B75" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C75" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="B76" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C76" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2336,21 +2967,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C20"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2358,10 +2994,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2369,10 +3005,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2380,10 +3016,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2391,10 +3027,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2402,10 +3038,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
         <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2413,10 +3049,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2424,10 +3060,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2435,10 +3071,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
         <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2446,10 +3082,10 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2457,10 +3093,10 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2468,10 +3104,10 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2479,10 +3115,10 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
         <v>28</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2490,10 +3126,10 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2501,10 +3137,10 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2512,10 +3148,10 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2523,10 +3159,10 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2534,10 +3170,10 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2545,10 +3181,10 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
         <v>28</v>
-      </c>
-      <c r="C19" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2556,10 +3192,10 @@
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2575,12 +3211,108 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>